<commit_message>
random changes to syncronsise with version used in fits
</commit_message>
<xml_diff>
--- a/macros/multijet/mc_weights_multijet.xlsx
+++ b/macros/multijet/mc_weights_multijet.xlsx
@@ -274,8 +274,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -381,7 +441,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -426,6 +486,36 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -470,19 +560,39 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -820,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25:AA32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -919,13 +1029,13 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2">
-        <v>5000</v>
+        <v>19300</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2">
-        <v>234</v>
+        <v>225.2</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -937,8 +1047,8 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f>($A$2*$C2*F2)/(E2)</f>
-        <v>0.16922020437172444</v>
+        <f t="shared" ref="G2:G13" si="0">($A$2*$C2*F2)/(E2)</f>
+        <v>0.62862557903682748</v>
       </c>
       <c r="H2">
         <v>29018</v>
@@ -972,43 +1082,43 @@
       </c>
       <c r="R2" s="8">
         <f>H2*$G2</f>
-        <v>4910.4318904586999</v>
+        <v>18241.457052490659</v>
       </c>
       <c r="S2" s="8">
-        <f t="shared" ref="S2:AA13" si="0">I2*$G2</f>
-        <v>8332.7413036724556</v>
+        <f t="shared" ref="S2:AA13" si="1">I2*$G2</f>
+        <v>30954.780762931459</v>
       </c>
       <c r="T2" s="8">
-        <f t="shared" si="0"/>
-        <v>184.9576833782948</v>
+        <f t="shared" si="1"/>
+        <v>687.08775788725245</v>
       </c>
       <c r="U2" s="8">
-        <f t="shared" si="0"/>
-        <v>187.83442685261414</v>
+        <f t="shared" si="1"/>
+        <v>697.7743927308785</v>
       </c>
       <c r="V2" s="8">
-        <f t="shared" si="0"/>
-        <v>67.180421135574605</v>
+        <f t="shared" si="1"/>
+        <v>249.5643548776205</v>
       </c>
       <c r="W2" s="8">
-        <f t="shared" si="0"/>
-        <v>39.089867209868345</v>
+        <f t="shared" si="1"/>
+        <v>145.21250875750715</v>
       </c>
       <c r="X2" s="8">
-        <f t="shared" si="0"/>
-        <v>5442.6294332077732</v>
+        <f t="shared" si="1"/>
+        <v>20218.484498561484</v>
       </c>
       <c r="Y2" s="8">
-        <f t="shared" si="0"/>
-        <v>6559.6520022655259</v>
+        <f t="shared" si="1"/>
+        <v>24368.041945783581</v>
       </c>
       <c r="Z2" s="8">
-        <f t="shared" si="0"/>
-        <v>231.66245978489076</v>
+        <f t="shared" si="1"/>
+        <v>860.5884177014168</v>
       </c>
       <c r="AA2" s="8">
-        <f t="shared" si="0"/>
-        <v>281.75164027892117</v>
+        <f t="shared" si="1"/>
+        <v>1046.6615890963178</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -1028,8 +1138,8 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>($A$2*$C3*F3)/(E3)</f>
-        <v>7.3491172197165569E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.28367592468105912</v>
       </c>
       <c r="H3">
         <v>29214</v>
@@ -1062,44 +1172,44 @@
         <v>1</v>
       </c>
       <c r="R3" s="8">
-        <f t="shared" ref="R3:R13" si="1">H3*$G3</f>
-        <v>2146.9711045679951</v>
+        <f t="shared" ref="R3:R13" si="2">H3*$G3</f>
+        <v>8287.308463632462</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" si="0"/>
-        <v>220.98795479687686</v>
+        <f t="shared" si="1"/>
+        <v>853.01350551594476</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" si="0"/>
-        <v>2404.9986101522431</v>
+        <f t="shared" si="1"/>
+        <v>9283.2946351876599</v>
       </c>
       <c r="U3" s="8">
-        <f t="shared" si="0"/>
-        <v>165.50211978801687</v>
+        <f t="shared" si="1"/>
+        <v>638.83818238174513</v>
       </c>
       <c r="V3" s="8">
-        <f t="shared" si="0"/>
-        <v>49.018611855509434</v>
+        <f t="shared" si="1"/>
+        <v>189.21184176226643</v>
       </c>
       <c r="W3" s="8">
-        <f t="shared" si="0"/>
-        <v>3.3805939210696163</v>
+        <f t="shared" si="1"/>
+        <v>13.04909253532872</v>
       </c>
       <c r="X3" s="8">
-        <f t="shared" si="0"/>
-        <v>0.80840289416882127</v>
+        <f t="shared" si="1"/>
+        <v>3.1204351714916503</v>
       </c>
       <c r="Y3" s="8">
-        <f t="shared" si="0"/>
-        <v>0.22047351659149672</v>
+        <f t="shared" si="1"/>
+        <v>0.85102777404317731</v>
       </c>
       <c r="Z3" s="8">
-        <f t="shared" si="0"/>
-        <v>1.6168057883376425</v>
+        <f t="shared" si="1"/>
+        <v>6.2408703429833006</v>
       </c>
       <c r="AA3" s="8">
-        <f t="shared" si="0"/>
-        <v>7.3491172197165569E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.28367592468105912</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -1119,8 +1229,8 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f>($A$2*$C4*F4)/(E4)</f>
-        <v>1066.8537079530402</v>
+        <f t="shared" si="0"/>
+        <v>4118.0553126987352</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1153,43 +1263,43 @@
         <v>0</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" si="1"/>
-        <v>2133.7074159060803</v>
+        <f t="shared" si="2"/>
+        <v>8236.1106253974704</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" si="0"/>
-        <v>1066.8537079530402</v>
+        <f t="shared" si="1"/>
+        <v>4118.0553126987352</v>
       </c>
       <c r="T4" s="8">
-        <f t="shared" si="0"/>
-        <v>10668.537079530401</v>
+        <f t="shared" si="1"/>
+        <v>41180.553126987354</v>
       </c>
       <c r="U4" s="8">
-        <f t="shared" si="0"/>
-        <v>2133.7074159060803</v>
+        <f t="shared" si="1"/>
+        <v>8236.1106253974704</v>
       </c>
       <c r="V4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1210,8 +1320,8 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f>($A$2*$C5*F5)/(E5)</f>
-        <v>51.055696770597692</v>
+        <f t="shared" si="0"/>
+        <v>197.0749895345071</v>
       </c>
       <c r="H5">
         <v>730</v>
@@ -1244,43 +1354,43 @@
         <v>0</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="1"/>
-        <v>37270.658642536313</v>
+        <f t="shared" si="2"/>
+        <v>143864.74236019017</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="0"/>
-        <v>13325.536857125997</v>
+        <f t="shared" si="1"/>
+        <v>51436.572268506352</v>
       </c>
       <c r="T5" s="8">
-        <f t="shared" si="0"/>
-        <v>57335.547473381208</v>
+        <f t="shared" si="1"/>
+        <v>221315.21324725146</v>
       </c>
       <c r="U5" s="8">
-        <f t="shared" si="0"/>
-        <v>18533.217927726961</v>
+        <f t="shared" si="1"/>
+        <v>71538.22120102607</v>
       </c>
       <c r="V5" s="8">
-        <f t="shared" si="0"/>
-        <v>765.83545155896536</v>
+        <f t="shared" si="1"/>
+        <v>2956.1248430176065</v>
       </c>
       <c r="W5" s="8">
-        <f t="shared" si="0"/>
-        <v>306.33418062358612</v>
+        <f t="shared" si="1"/>
+        <v>1182.4499372070427</v>
       </c>
       <c r="X5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z5" s="8">
-        <f t="shared" si="0"/>
-        <v>153.16709031179306</v>
+        <f t="shared" si="1"/>
+        <v>591.22496860352135</v>
       </c>
       <c r="AA5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1302,8 +1412,8 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f>($A$2*$C6*F6)/(E6)</f>
-        <v>1.3061259819739113</v>
+        <f t="shared" si="0"/>
+        <v>5.0416462904192976</v>
       </c>
       <c r="H6">
         <v>36576</v>
@@ -1336,44 +1446,44 @@
         <v>4</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" si="1"/>
-        <v>47772.863916677779</v>
+        <f t="shared" si="2"/>
+        <v>184403.25471837624</v>
       </c>
       <c r="S6" s="8">
-        <f t="shared" si="0"/>
-        <v>11966.726246844975</v>
+        <f t="shared" si="1"/>
+        <v>46191.563312821607</v>
       </c>
       <c r="T6" s="8">
-        <f t="shared" si="0"/>
-        <v>68369.164526424385</v>
+        <f t="shared" si="1"/>
+        <v>263904.97507199814</v>
       </c>
       <c r="U6" s="8">
-        <f t="shared" si="0"/>
-        <v>13953.343865427294</v>
+        <f t="shared" si="1"/>
+        <v>53859.907320549355</v>
       </c>
       <c r="V6" s="8">
-        <f t="shared" si="0"/>
-        <v>1259.1054466228504</v>
+        <f t="shared" si="1"/>
+        <v>4860.1470239642031</v>
       </c>
       <c r="W6" s="8">
-        <f t="shared" si="0"/>
-        <v>227.26592086346056</v>
+        <f t="shared" si="1"/>
+        <v>877.24645453295773</v>
       </c>
       <c r="X6" s="8">
-        <f t="shared" si="0"/>
-        <v>28.734771603426047</v>
+        <f t="shared" si="1"/>
+        <v>110.91621838922455</v>
       </c>
       <c r="Y6" s="8">
-        <f t="shared" si="0"/>
-        <v>20.89801571158258</v>
+        <f t="shared" si="1"/>
+        <v>80.666340646708761</v>
       </c>
       <c r="Z6" s="8">
-        <f t="shared" si="0"/>
-        <v>44.408283387112981</v>
+        <f t="shared" si="1"/>
+        <v>171.41597387425611</v>
       </c>
       <c r="AA6" s="8">
-        <f t="shared" si="0"/>
-        <v>5.2245039278956451</v>
+        <f t="shared" si="1"/>
+        <v>20.16658516167719</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1393,8 +1503,8 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>($A$2*$C7*F7)/(E7)</f>
-        <v>3.2813755809178171</v>
+        <f t="shared" si="0"/>
+        <v>12.666109742342774</v>
       </c>
       <c r="H7">
         <v>52</v>
@@ -1427,44 +1537,44 @@
         <v>565</v>
       </c>
       <c r="R7" s="8">
-        <f t="shared" si="1"/>
-        <v>170.63153020772648</v>
+        <f t="shared" si="2"/>
+        <v>658.63770660182422</v>
       </c>
       <c r="S7" s="8">
-        <f t="shared" si="0"/>
-        <v>32.813755809178168</v>
+        <f t="shared" si="1"/>
+        <v>126.66109742342775</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" si="0"/>
-        <v>298.60517786352136</v>
+        <f t="shared" si="1"/>
+        <v>1152.6159865531924</v>
       </c>
       <c r="U7" s="8">
-        <f t="shared" si="0"/>
-        <v>68.908887199274162</v>
+        <f t="shared" si="1"/>
+        <v>265.98830458919826</v>
       </c>
       <c r="V7" s="8">
-        <f t="shared" si="0"/>
-        <v>150.94327672221959</v>
+        <f t="shared" si="1"/>
+        <v>582.64104814776761</v>
       </c>
       <c r="W7" s="8">
-        <f t="shared" si="0"/>
-        <v>75.471638361109797</v>
+        <f t="shared" si="1"/>
+        <v>291.3205240738838</v>
       </c>
       <c r="X7" s="8">
-        <f t="shared" si="0"/>
-        <v>462.6739569094122</v>
+        <f t="shared" si="1"/>
+        <v>1785.9214736703311</v>
       </c>
       <c r="Y7" s="8">
-        <f t="shared" si="0"/>
-        <v>607.0544824697962</v>
+        <f t="shared" si="1"/>
+        <v>2343.2303023334134</v>
       </c>
       <c r="Z7" s="8">
-        <f t="shared" si="0"/>
-        <v>1578.3416544214701</v>
+        <f t="shared" si="1"/>
+        <v>6092.3987860668749</v>
       </c>
       <c r="AA7" s="8">
-        <f t="shared" si="0"/>
-        <v>1853.9772032185667</v>
+        <f t="shared" si="1"/>
+        <v>7156.3520044236675</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1485,8 +1595,8 @@
         <v>0.996</v>
       </c>
       <c r="G8">
-        <f>($A$2*$C8*F8)/(E8)</f>
-        <v>0.11107628130161677</v>
+        <f t="shared" si="0"/>
+        <v>0.42875444582424072</v>
       </c>
       <c r="H8">
         <v>966</v>
@@ -1519,44 +1629,44 @@
         <v>105</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" si="1"/>
-        <v>107.29968773736181</v>
+        <f t="shared" si="2"/>
+        <v>414.17679466621655</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" si="0"/>
-        <v>132.62507987413042</v>
+        <f t="shared" si="1"/>
+        <v>511.93280831414341</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" si="0"/>
-        <v>5.5538140650808385</v>
+        <f t="shared" si="1"/>
+        <v>21.437722291212037</v>
       </c>
       <c r="U8" s="8">
-        <f t="shared" si="0"/>
-        <v>6.4424243154937724</v>
+        <f t="shared" si="1"/>
+        <v>24.867757857805962</v>
       </c>
       <c r="V8" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1107628130161677</v>
+        <f t="shared" si="1"/>
+        <v>4.2875444582424072</v>
       </c>
       <c r="W8" s="8">
-        <f t="shared" si="0"/>
-        <v>0.88861025041293418</v>
+        <f t="shared" si="1"/>
+        <v>3.4300355665939257</v>
       </c>
       <c r="X8" s="8">
-        <f t="shared" si="0"/>
-        <v>123.183595963493</v>
+        <f t="shared" si="1"/>
+        <v>475.48868041908293</v>
       </c>
       <c r="Y8" s="8">
-        <f t="shared" si="0"/>
-        <v>146.06530991162606</v>
+        <f t="shared" si="1"/>
+        <v>563.81209625887652</v>
       </c>
       <c r="Z8" s="8">
-        <f t="shared" si="0"/>
-        <v>11.440856974066527</v>
+        <f t="shared" si="1"/>
+        <v>44.161707919896791</v>
       </c>
       <c r="AA8" s="8">
-        <f t="shared" si="0"/>
-        <v>11.663009536669762</v>
+        <f t="shared" si="1"/>
+        <v>45.019216811545277</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1577,8 +1687,8 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <f>($A$2*$C9*F9)/(E9)</f>
-        <v>0.11247112227941475</v>
+        <f t="shared" si="0"/>
+        <v>0.43413853199854091</v>
       </c>
       <c r="H9">
         <v>911</v>
@@ -1611,44 +1721,44 @@
         <v>91</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" si="1"/>
-        <v>102.46119239654683</v>
+        <f t="shared" si="2"/>
+        <v>395.50020265067076</v>
       </c>
       <c r="S9" s="8">
-        <f t="shared" si="0"/>
-        <v>126.64248368662101</v>
+        <f t="shared" si="1"/>
+        <v>488.83998703035707</v>
       </c>
       <c r="T9" s="8">
-        <f t="shared" si="0"/>
-        <v>5.8484983585295671</v>
+        <f t="shared" si="1"/>
+        <v>22.575203663924128</v>
       </c>
       <c r="U9" s="8">
-        <f t="shared" si="0"/>
-        <v>6.1859117253678111</v>
+        <f t="shared" si="1"/>
+        <v>23.877619259919751</v>
       </c>
       <c r="V9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.4621245896323918</v>
+        <f t="shared" si="1"/>
+        <v>5.6438009159810321</v>
       </c>
       <c r="W9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.1247112227941476</v>
+        <f t="shared" si="1"/>
+        <v>4.3413853199854096</v>
       </c>
       <c r="X9" s="8">
-        <f t="shared" si="0"/>
-        <v>122.48105216228267</v>
+        <f t="shared" si="1"/>
+        <v>472.77686134641107</v>
       </c>
       <c r="Y9" s="8">
-        <f t="shared" si="0"/>
-        <v>140.2514894824302</v>
+        <f t="shared" si="1"/>
+        <v>541.37074940218054</v>
       </c>
       <c r="Z9" s="8">
-        <f t="shared" si="0"/>
-        <v>8.4353341709561054</v>
+        <f t="shared" si="1"/>
+        <v>32.560389899890566</v>
       </c>
       <c r="AA9" s="8">
-        <f t="shared" si="0"/>
-        <v>10.234872127426742</v>
+        <f t="shared" si="1"/>
+        <v>39.506606411867224</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1668,8 +1778,8 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>($A$2*$C10*F10)/(E10)</f>
-        <v>0.57608565866329109</v>
+        <f t="shared" si="0"/>
+        <v>2.2236906424403036</v>
       </c>
       <c r="H10">
         <v>26</v>
@@ -1702,44 +1812,44 @@
         <v>84</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" si="1"/>
-        <v>14.978227125245569</v>
+        <f t="shared" si="2"/>
+        <v>57.815956703447895</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" si="0"/>
-        <v>6.9130279039594935</v>
+        <f t="shared" si="1"/>
+        <v>26.684287709283645</v>
       </c>
       <c r="T10" s="8">
-        <f t="shared" si="0"/>
-        <v>6.9130279039594935</v>
+        <f t="shared" si="1"/>
+        <v>26.684287709283645</v>
       </c>
       <c r="U10" s="8">
-        <f t="shared" si="0"/>
-        <v>7.4891135626227845</v>
+        <f t="shared" si="1"/>
+        <v>28.907978351723948</v>
       </c>
       <c r="V10" s="8">
-        <f t="shared" si="0"/>
-        <v>2.3043426346531644</v>
+        <f t="shared" si="1"/>
+        <v>8.8947625697612143</v>
       </c>
       <c r="W10" s="8">
-        <f t="shared" si="0"/>
-        <v>1.7282569759898734</v>
+        <f t="shared" si="1"/>
+        <v>6.6710719273209111</v>
       </c>
       <c r="X10" s="8">
-        <f t="shared" si="0"/>
-        <v>17.858655418562023</v>
+        <f t="shared" si="1"/>
+        <v>68.934409915649411</v>
       </c>
       <c r="Y10" s="8">
-        <f t="shared" si="0"/>
-        <v>19.586912394551899</v>
+        <f t="shared" si="1"/>
+        <v>75.60548184297032</v>
       </c>
       <c r="Z10" s="8">
-        <f t="shared" si="0"/>
-        <v>35.141225178460758</v>
+        <f t="shared" si="1"/>
+        <v>135.6451291888585</v>
       </c>
       <c r="AA10" s="8">
-        <f t="shared" si="0"/>
-        <v>48.391195327716453</v>
+        <f t="shared" si="1"/>
+        <v>186.79001396498549</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1759,8 +1869,8 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>($A$2*$C11*F11)/(E11)</f>
-        <v>2.7507433648436358E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.10617869388296433</v>
       </c>
       <c r="H11">
         <v>340</v>
@@ -1793,44 +1903,44 @@
         <v>771</v>
       </c>
       <c r="R11" s="8">
-        <f t="shared" si="1"/>
-        <v>9.3525274404683625</v>
+        <f t="shared" si="2"/>
+        <v>36.100755920207874</v>
       </c>
       <c r="S11" s="8">
-        <f t="shared" si="0"/>
-        <v>6.5192617746794168</v>
+        <f t="shared" si="1"/>
+        <v>25.164350450262546</v>
       </c>
       <c r="T11" s="8">
-        <f t="shared" si="0"/>
-        <v>8.3622598291246533</v>
+        <f t="shared" si="1"/>
+        <v>32.278322940421155</v>
       </c>
       <c r="U11" s="8">
-        <f t="shared" si="0"/>
-        <v>6.5192617746794168</v>
+        <f t="shared" si="1"/>
+        <v>25.164350450262546</v>
       </c>
       <c r="V11" s="8">
-        <f t="shared" si="0"/>
-        <v>1.4303865497186905</v>
+        <f t="shared" si="1"/>
+        <v>5.5212920819141456</v>
       </c>
       <c r="W11" s="8">
-        <f t="shared" si="0"/>
-        <v>0.96276017769527256</v>
+        <f t="shared" si="1"/>
+        <v>3.7162542859037515</v>
       </c>
       <c r="X11" s="8">
-        <f t="shared" si="0"/>
-        <v>9.3800348741167987</v>
+        <f t="shared" si="1"/>
+        <v>36.206934614090834</v>
       </c>
       <c r="Y11" s="8">
-        <f t="shared" si="0"/>
-        <v>10.232765317218325</v>
+        <f t="shared" si="1"/>
+        <v>39.498474124462732</v>
       </c>
       <c r="Z11" s="8">
-        <f t="shared" si="0"/>
-        <v>16.256893286225889</v>
+        <f t="shared" si="1"/>
+        <v>62.751608084831922</v>
       </c>
       <c r="AA11" s="8">
-        <f t="shared" si="0"/>
-        <v>21.208231342944433</v>
+        <f t="shared" si="1"/>
+        <v>81.8637729837655</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1850,8 +1960,8 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>($A$2*$C12*F12)/(E12)</f>
-        <v>1.6604530091798402E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.4093486154341836E-2</v>
       </c>
       <c r="H12">
         <v>564</v>
@@ -1884,44 +1994,44 @@
         <v>474</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" si="1"/>
-        <v>9.3649549717742993</v>
+        <f t="shared" si="2"/>
+        <v>36.148726191048794</v>
       </c>
       <c r="S12" s="8">
-        <f t="shared" si="0"/>
-        <v>6.6086029765357637</v>
+        <f t="shared" si="1"/>
+        <v>25.50920748942805</v>
       </c>
       <c r="T12" s="8">
-        <f t="shared" si="0"/>
-        <v>6.0440489534146185</v>
+        <f t="shared" si="1"/>
+        <v>23.330028960180428</v>
       </c>
       <c r="U12" s="8">
-        <f t="shared" si="0"/>
-        <v>4.2839687636839878</v>
+        <f t="shared" si="1"/>
+        <v>16.536119427820193</v>
       </c>
       <c r="V12" s="8">
-        <f t="shared" si="0"/>
-        <v>0.74720385413092805</v>
+        <f t="shared" si="1"/>
+        <v>2.8842068769453828</v>
       </c>
       <c r="W12" s="8">
-        <f t="shared" si="0"/>
-        <v>0.26567248146877442</v>
+        <f t="shared" si="1"/>
+        <v>1.0254957784694694</v>
       </c>
       <c r="X12" s="8">
-        <f t="shared" si="0"/>
-        <v>6.1270716038736097</v>
+        <f t="shared" si="1"/>
+        <v>23.650496390952139</v>
       </c>
       <c r="Y12" s="8">
-        <f t="shared" si="0"/>
-        <v>6.4093486154341832</v>
+        <f t="shared" si="1"/>
+        <v>24.74008565557595</v>
       </c>
       <c r="Z12" s="8">
-        <f t="shared" si="0"/>
-        <v>6.6418120367193607</v>
+        <f t="shared" si="1"/>
+        <v>25.637394461736733</v>
       </c>
       <c r="AA12" s="8">
-        <f t="shared" si="0"/>
-        <v>7.8705472635124423</v>
+        <f t="shared" si="1"/>
+        <v>30.380312437158029</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1941,8 +2051,8 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f>($A$2*$C13*F13)/(E13)</f>
-        <v>9.0181615782385545E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.481010369200082E-2</v>
       </c>
       <c r="H13">
         <v>771</v>
@@ -1975,44 +2085,44 @@
         <v>52</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" si="1"/>
-        <v>6.9530025768219259</v>
+        <f t="shared" si="2"/>
+        <v>26.838589946532633</v>
       </c>
       <c r="S13" s="8">
-        <f t="shared" si="0"/>
-        <v>4.7615893133099565</v>
+        <f t="shared" si="1"/>
+        <v>18.379734749376432</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" si="0"/>
-        <v>3.1834110371182098</v>
+        <f t="shared" si="1"/>
+        <v>12.28796660327629</v>
       </c>
       <c r="U13" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0561408398383905</v>
+        <f t="shared" si="1"/>
+        <v>7.9367036417761865</v>
       </c>
       <c r="V13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.18938139314300964</v>
+        <f t="shared" si="1"/>
+        <v>0.73101217753201719</v>
       </c>
       <c r="W13" s="8">
-        <f t="shared" si="0"/>
-        <v>9.9199777360624103E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.38291114061200904</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.6042168257419831</v>
+        <f t="shared" si="1"/>
+        <v>2.332276947364055</v>
       </c>
       <c r="Y13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.55912601785079041</v>
+        <f t="shared" si="1"/>
+        <v>2.1582264289040509</v>
       </c>
       <c r="Z13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.51403520995959762</v>
+        <f t="shared" si="1"/>
+        <v>1.9841759104440466</v>
       </c>
       <c r="AA13" s="8">
-        <f t="shared" si="0"/>
-        <v>0.46894440206840482</v>
+        <f t="shared" si="1"/>
+        <v>1.8101253919840425</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -2057,43 +2167,43 @@
     <row r="17" spans="2:28">
       <c r="R17" s="8">
         <f>SUM(R2:R13)</f>
-        <v>94655.674092602814</v>
+        <v>364658.09195276693</v>
       </c>
       <c r="S17" s="8">
-        <f t="shared" ref="S17:AA17" si="2">SUM(S2:S13)</f>
-        <v>35229.729871731761</v>
+        <f t="shared" ref="S17:AA17" si="3">SUM(S2:S13)</f>
+        <v>134777.15663564039</v>
       </c>
       <c r="T17" s="8">
-        <f t="shared" si="2"/>
-        <v>139297.71561087732</v>
+        <f t="shared" si="3"/>
+        <v>537662.33335803333</v>
       </c>
       <c r="U17" s="8">
-        <f t="shared" si="2"/>
-        <v>35075.491463881917</v>
+        <f t="shared" si="3"/>
+        <v>135364.13055566407</v>
       </c>
       <c r="V17" s="8">
-        <f t="shared" si="2"/>
-        <v>2299.3274097294138</v>
+        <f t="shared" si="3"/>
+        <v>8865.6517308498387</v>
       </c>
       <c r="W17" s="8">
-        <f t="shared" si="2"/>
-        <v>656.6114118648162</v>
+        <f t="shared" si="3"/>
+        <v>2528.8456711256063</v>
       </c>
       <c r="X17" s="8">
-        <f t="shared" si="2"/>
-        <v>6214.4811914628508</v>
+        <f t="shared" si="3"/>
+        <v>23197.832285426084</v>
       </c>
       <c r="Y17" s="8">
-        <f t="shared" si="2"/>
-        <v>7510.9299257026087</v>
+        <f t="shared" si="3"/>
+        <v>28039.974730250713</v>
       </c>
       <c r="Z17" s="8">
-        <f t="shared" si="2"/>
-        <v>2087.626450549993</v>
+        <f t="shared" si="3"/>
+        <v>8024.609422054712</v>
       </c>
       <c r="AA17" s="8">
-        <f t="shared" si="2"/>
-        <v>2240.8636385979189</v>
+        <f t="shared" si="3"/>
+        <v>8608.8339026076483</v>
       </c>
     </row>
     <row r="18" spans="2:28">
@@ -2105,43 +2215,43 @@
       </c>
       <c r="R18" s="8">
         <f>SUM(R3:R6)*$Q$18 + (SUM(R2:R12)-SUM(R3:R6))</f>
-        <v>94648.721090025996</v>
+        <v>364631.25336282043</v>
       </c>
       <c r="S18" s="8">
-        <f t="shared" ref="S18:AA18" si="3">SUM(S3:S6)*$Q$18 + (SUM(S2:S12)-SUM(S3:S6))</f>
-        <v>35224.968282418449</v>
+        <f t="shared" ref="S18:AA18" si="4">SUM(S3:S6)*$Q$18 + (SUM(S2:S12)-SUM(S3:S6))</f>
+        <v>134758.77690089101</v>
       </c>
       <c r="T18" s="8">
-        <f t="shared" si="3"/>
-        <v>139294.53219984021</v>
+        <f t="shared" si="4"/>
+        <v>537650.04539143003</v>
       </c>
       <c r="U18" s="8">
-        <f t="shared" si="3"/>
-        <v>35073.435323042082</v>
+        <f t="shared" si="4"/>
+        <v>135356.19385202229</v>
       </c>
       <c r="V18" s="8">
-        <f t="shared" si="3"/>
-        <v>2299.138028336271</v>
+        <f t="shared" si="4"/>
+        <v>8864.920718672307</v>
       </c>
       <c r="W18" s="8">
-        <f t="shared" si="3"/>
-        <v>656.51221208745562</v>
+        <f t="shared" si="4"/>
+        <v>2528.4627599849941</v>
       </c>
       <c r="X18" s="8">
-        <f t="shared" si="3"/>
-        <v>6213.876974637109</v>
+        <f t="shared" si="4"/>
+        <v>23195.500008478721</v>
       </c>
       <c r="Y18" s="8">
-        <f t="shared" si="3"/>
-        <v>7510.3707996847579</v>
+        <f t="shared" si="4"/>
+        <v>28037.81650382181</v>
       </c>
       <c r="Z18" s="8">
-        <f t="shared" si="3"/>
-        <v>2087.1124153400333</v>
+        <f t="shared" si="4"/>
+        <v>8022.6252461442682</v>
       </c>
       <c r="AA18" s="8">
-        <f t="shared" si="3"/>
-        <v>2240.3946941958507</v>
+        <f t="shared" si="4"/>
+        <v>8607.0237772156634</v>
       </c>
     </row>
     <row r="19" spans="2:28">
@@ -2207,43 +2317,43 @@
       </c>
       <c r="R21" s="10">
         <f>R19/R17</f>
-        <v>0.97943415319510208</v>
+        <v>0.25423541132335087</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" ref="S21:AA21" si="4">S19/S17</f>
-        <v>1.1688423428145873</v>
+        <f t="shared" ref="S21:AA21" si="5">S19/S17</f>
+        <v>0.3055265523320212</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="4"/>
-        <v>0.65107313212046725</v>
+        <f t="shared" si="5"/>
+        <v>0.16868021874168906</v>
       </c>
       <c r="U21" s="10">
-        <f t="shared" si="4"/>
-        <v>0.86179833092649616</v>
+        <f t="shared" si="5"/>
+        <v>0.22330878849452457</v>
       </c>
       <c r="V21" s="10">
-        <f t="shared" si="4"/>
-        <v>1.3991047931614831</v>
+        <f t="shared" si="5"/>
+        <v>0.36286108429071201</v>
       </c>
       <c r="W21" s="10">
-        <f t="shared" si="4"/>
-        <v>1.6691759847537428</v>
+        <f t="shared" si="5"/>
+        <v>0.43339932227345568</v>
       </c>
       <c r="X21" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1124017897900698</v>
+        <f t="shared" si="5"/>
+        <v>0.298001982036186</v>
       </c>
       <c r="Y21" s="10">
-        <f t="shared" si="4"/>
-        <v>1.1033254313346286</v>
+        <f t="shared" si="5"/>
+        <v>0.29554234908277693</v>
       </c>
       <c r="Z21" s="10">
-        <f t="shared" si="4"/>
-        <v>0.88952695512684576</v>
+        <f t="shared" si="5"/>
+        <v>0.23141313207048433</v>
       </c>
       <c r="AA21" s="10">
-        <f t="shared" si="4"/>
-        <v>0.98890443926633764</v>
+        <f t="shared" si="5"/>
+        <v>0.25741000756545729</v>
       </c>
     </row>
     <row r="22" spans="2:28">
@@ -2252,43 +2362,43 @@
       </c>
       <c r="R22" s="10">
         <f>SUM(R3:R6)/R17</f>
-        <v>0.94367508272458345</v>
+        <v>0.94551971772028076</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" ref="S22:AA22" si="5">SUM(S3:S6)/S17</f>
-        <v>0.7544793804407991</v>
+        <f t="shared" ref="S22:AA22" si="6">SUM(S3:S6)/S17</f>
+        <v>0.76125069678470547</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="5"/>
-        <v>0.99627080803794221</v>
+        <f t="shared" si="6"/>
+        <v>0.99632055817588527</v>
       </c>
       <c r="U22" s="10">
-        <f t="shared" si="5"/>
-        <v>0.99174009763107951</v>
+        <f t="shared" si="6"/>
+        <v>0.99193986455768823</v>
       </c>
       <c r="V22" s="10">
-        <f t="shared" si="5"/>
-        <v>0.90198529416103912</v>
+        <f t="shared" si="6"/>
+        <v>0.90297746311050842</v>
       </c>
       <c r="W22" s="10">
-        <f t="shared" si="5"/>
-        <v>0.81780591336824093</v>
+        <f t="shared" si="6"/>
+        <v>0.81964095632326039</v>
       </c>
       <c r="X22" s="10">
-        <f t="shared" si="5"/>
-        <v>4.7539245171712534E-3</v>
+        <f t="shared" si="6"/>
+        <v>4.9158323138821522E-3</v>
       </c>
       <c r="Y22" s="10">
-        <f t="shared" si="5"/>
-        <v>2.8117010060107238E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.9071840900344158E-3</v>
       </c>
       <c r="Z22" s="10">
-        <f t="shared" si="5"/>
-        <v>9.5415623534931632E-2</v>
+        <f t="shared" si="6"/>
+        <v>9.5815481150718418E-2</v>
       </c>
       <c r="AA22" s="10">
-        <f t="shared" si="5"/>
-        <v>2.3642648346990456E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.3754972296728583E-3</v>
       </c>
     </row>
     <row r="23" spans="2:28">
@@ -2297,43 +2407,43 @@
       </c>
       <c r="R23" s="10">
         <f>R$2/R17</f>
-        <v>5.1876783272968546E-2</v>
+        <v>5.0023453352718746E-2</v>
       </c>
       <c r="S23" s="10">
-        <f t="shared" ref="S23:AA23" si="6">S$2/S17</f>
-        <v>0.23652583582137041</v>
+        <f t="shared" ref="S23:AA23" si="7">S$2/S17</f>
+        <v>0.22967379291592649</v>
       </c>
       <c r="T23" s="10">
-        <f t="shared" si="6"/>
-        <v>1.3277869099803962E-3</v>
+        <f t="shared" si="7"/>
+        <v>1.2779168546101511E-3</v>
       </c>
       <c r="U23" s="10">
-        <f t="shared" si="6"/>
-        <v>5.3551473981777791E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.1547953646696792E-3</v>
       </c>
       <c r="V23" s="10">
-        <f t="shared" si="6"/>
-        <v>2.9217422821693949E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.8149577995401125E-2</v>
       </c>
       <c r="W23" s="10">
-        <f t="shared" si="6"/>
-        <v>5.953272590686591E-2</v>
+        <f t="shared" si="7"/>
+        <v>5.7422447884244388E-2</v>
       </c>
       <c r="X23" s="10">
-        <f t="shared" si="6"/>
-        <v>0.87579787685005639</v>
+        <f t="shared" si="7"/>
+        <v>0.87156783658892301</v>
       </c>
       <c r="Y23" s="10">
-        <f t="shared" si="6"/>
-        <v>0.87334751717203707</v>
+        <f t="shared" si="7"/>
+        <v>0.86904650165373742</v>
       </c>
       <c r="Z23" s="10">
-        <f t="shared" si="6"/>
-        <v>0.11096930666109275</v>
+        <f t="shared" si="7"/>
+        <v>0.10724365167682666</v>
       </c>
       <c r="AA23" s="10">
-        <f t="shared" si="6"/>
-        <v>0.12573350534404215</v>
+        <f t="shared" si="7"/>
+        <v>0.12157994926342812</v>
       </c>
     </row>
     <row r="24" spans="2:28">
@@ -2392,48 +2502,48 @@
         <v>17</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" ref="R25:R27" si="7">(H25/$E25)*100</f>
+        <f t="shared" ref="R25" si="8">(H25/$E25)*100</f>
         <v>0.47200944018880375</v>
       </c>
       <c r="S25" s="6">
-        <f t="shared" ref="S25" si="8">(I25/$E25)*100</f>
+        <f t="shared" ref="S25" si="9">(I25/$E25)*100</f>
         <v>1.0820216404328087</v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" ref="T25" si="9">(J25/$E25)*100</f>
+        <f t="shared" ref="T25" si="10">(J25/$E25)*100</f>
         <v>1.6000320006400129E-2</v>
       </c>
       <c r="U25" s="6">
-        <f t="shared" ref="U25" si="10">(K25/$E25)*100</f>
+        <f t="shared" ref="U25" si="11">(K25/$E25)*100</f>
         <v>2.8000560011200226E-2</v>
       </c>
       <c r="V25" s="6">
-        <f t="shared" ref="V25" si="11">(L25/$E25)*100</f>
+        <f t="shared" ref="V25" si="12">(L25/$E25)*100</f>
         <v>0</v>
       </c>
       <c r="W25" s="6">
-        <f t="shared" ref="W25" si="12">(M25/$E25)*100</f>
+        <f t="shared" ref="W25" si="13">(M25/$E25)*100</f>
         <v>2.0000400008000161E-3</v>
       </c>
       <c r="X25" s="6">
-        <f t="shared" ref="X25" si="13">(N25/$E25)*100</f>
+        <f t="shared" ref="X25" si="14">(N25/$E25)*100</f>
         <v>0.38800776015520311</v>
       </c>
       <c r="Y25" s="6">
-        <f t="shared" ref="Y25" si="14">(O25/$E25)*100</f>
+        <f t="shared" ref="Y25" si="15">(O25/$E25)*100</f>
         <v>0.54801096021920437</v>
       </c>
       <c r="Z25" s="6">
-        <f t="shared" ref="Z25" si="15">(P25/$E25)*100</f>
+        <f t="shared" ref="Z25" si="16">(P25/$E25)*100</f>
         <v>1.2000240004800097E-2</v>
       </c>
       <c r="AA25" s="6">
-        <f t="shared" ref="AA25" si="16">(Q25/$E25)*100</f>
+        <f t="shared" ref="AA25" si="17">(Q25/$E25)*100</f>
         <v>3.4000680013600272E-2</v>
       </c>
       <c r="AB25">
         <f>((R25+S25+X25+Y25)/100)*$C25*$A$2</f>
-        <v>2306.3463769275381</v>
+        <v>8902.497014940298</v>
       </c>
     </row>
     <row r="26" spans="2:28">
@@ -2477,48 +2587,48 @@
         <v>71</v>
       </c>
       <c r="R26" s="6">
-        <f t="shared" ref="R26:R34" si="17">(H26/$E26)*100</f>
+        <f t="shared" ref="R26:R32" si="18">(H26/$E26)*100</f>
         <v>4.1925869621747047</v>
       </c>
       <c r="S26" s="6">
-        <f t="shared" ref="S26:S34" si="18">(I26/$E26)*100</f>
+        <f t="shared" ref="S26:S32" si="19">(I26/$E26)*100</f>
         <v>7.7410837517252418</v>
       </c>
       <c r="T26" s="6">
-        <f t="shared" ref="T26:T34" si="19">(J26/$E26)*100</f>
+        <f t="shared" ref="T26:T32" si="20">(J26/$E26)*100</f>
         <v>0.19602744384213791</v>
       </c>
       <c r="U26" s="6">
-        <f t="shared" ref="U26:U34" si="20">(K26/$E26)*100</f>
+        <f t="shared" ref="U26:U32" si="21">(K26/$E26)*100</f>
         <v>0.20602884403816535</v>
       </c>
       <c r="V26" s="6">
-        <f t="shared" ref="V26:V34" si="21">(L26/$E26)*100</f>
+        <f t="shared" ref="V26:V32" si="22">(L26/$E26)*100</f>
         <v>2.8003920548876841E-2</v>
       </c>
       <c r="W26" s="6">
-        <f t="shared" ref="W26:W34" si="22">(M26/$E26)*100</f>
+        <f t="shared" ref="W26:W32" si="23">(M26/$E26)*100</f>
         <v>3.2004480627287821E-2</v>
       </c>
       <c r="X26" s="6">
-        <f t="shared" ref="X26:X34" si="23">(N26/$E26)*100</f>
+        <f t="shared" ref="X26:X32" si="24">(N26/$E26)*100</f>
         <v>2.3943352069289698</v>
       </c>
       <c r="Y26" s="6">
-        <f t="shared" ref="Y26:Y34" si="24">(O26/$E26)*100</f>
+        <f t="shared" ref="Y26:Y32" si="25">(O26/$E26)*100</f>
         <v>3.1184365811213572</v>
       </c>
       <c r="Z26" s="6">
-        <f t="shared" ref="Z26:Z34" si="25">(P26/$E26)*100</f>
+        <f t="shared" ref="Z26:Z32" si="26">(P26/$E26)*100</f>
         <v>7.8010921529014066E-2</v>
       </c>
       <c r="AA26" s="6">
-        <f t="shared" ref="AA26:AA34" si="26">(Q26/$E26)*100</f>
+        <f t="shared" ref="AA26:AA32" si="27">(Q26/$E26)*100</f>
         <v>0.14201988278358971</v>
       </c>
       <c r="AB26">
-        <f t="shared" ref="AB26:AB32" si="27">((R26+S26+X26+Y26)/100)*$C26*$A$2</f>
-        <v>74.65742737983318</v>
+        <f t="shared" ref="AB26:AB32" si="28">((R26+S26+X26+Y26)/100)*$C26*$A$2</f>
+        <v>288.17766968615604</v>
       </c>
     </row>
     <row r="27" spans="2:28">
@@ -2562,48 +2672,48 @@
         <v>50</v>
       </c>
       <c r="R27" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.816305304424354</v>
       </c>
       <c r="S27" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.1365709256740546</v>
       </c>
       <c r="T27" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.15601248099847989</v>
       </c>
       <c r="U27" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.18001440115209216</v>
       </c>
       <c r="V27" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.0002400192015364E-2</v>
       </c>
       <c r="W27" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.6001280102408193E-2</v>
       </c>
       <c r="X27" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.0961676934154729</v>
       </c>
       <c r="Y27" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.7762220977678211</v>
       </c>
       <c r="Z27" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>8.4006720537643007E-2</v>
       </c>
       <c r="AA27" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.10000800064005121</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="27"/>
-        <v>67.720032242579407</v>
+        <f t="shared" si="28"/>
+        <v>261.39932445635651</v>
       </c>
     </row>
     <row r="28" spans="2:28">
@@ -2647,48 +2757,48 @@
         <v>75</v>
       </c>
       <c r="R28" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.0949170850753136</v>
       </c>
       <c r="S28" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8.3294993098757786</v>
       </c>
       <c r="T28" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.2400432077773999</v>
       </c>
       <c r="U28" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.18003240583304997</v>
       </c>
       <c r="V28" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.4004320777739993E-2</v>
       </c>
       <c r="W28" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>4.0007201296233322E-2</v>
       </c>
       <c r="X28" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.0125422576063694</v>
       </c>
       <c r="Y28" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.7546758416514976</v>
       </c>
       <c r="Z28" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.1240223240183233</v>
       </c>
       <c r="AA28" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.15002700486087495</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="27"/>
-        <v>12.65944812066172</v>
+        <f t="shared" si="28"/>
+        <v>48.86546974575424</v>
       </c>
     </row>
     <row r="29" spans="2:28">
@@ -2732,48 +2842,48 @@
         <v>66</v>
       </c>
       <c r="R29" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.1161646465858635</v>
       </c>
       <c r="S29" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.6882675307012276</v>
       </c>
       <c r="T29" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.1920076803072123</v>
       </c>
       <c r="U29" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.17200688027521102</v>
       </c>
       <c r="V29" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.800152006080243E-2</v>
       </c>
       <c r="W29" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.4000560022400896E-2</v>
       </c>
       <c r="X29" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.5841033641345654</v>
       </c>
       <c r="Y29" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.1781271250850036</v>
       </c>
       <c r="Z29" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>8.8003520140805633E-2</v>
       </c>
       <c r="AA29" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.13200528021120844</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="27"/>
-        <v>6.7211778771150854</v>
+        <f t="shared" si="28"/>
+        <v>25.943746605664227</v>
       </c>
     </row>
     <row r="30" spans="2:28">
@@ -2817,48 +2927,48 @@
         <v>71</v>
       </c>
       <c r="R30" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.1062463747824873</v>
       </c>
       <c r="S30" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.9124147448846927</v>
       </c>
       <c r="T30" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.22401344080644842</v>
       </c>
       <c r="U30" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.1560093605616337</v>
       </c>
       <c r="V30" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.4002040122407345E-2</v>
       </c>
       <c r="W30" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.4000840050403026E-2</v>
       </c>
       <c r="X30" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.5081504890293416</v>
       </c>
       <c r="Y30" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.1201872112326741</v>
       </c>
       <c r="Z30" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>7.600456027361642E-2</v>
       </c>
       <c r="AA30" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.14200852051123067</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="27"/>
-        <v>6.7537706562393751</v>
+        <f t="shared" si="28"/>
+        <v>26.069554733083987</v>
       </c>
     </row>
     <row r="31" spans="2:28">
@@ -2902,48 +3012,48 @@
         <v>63</v>
       </c>
       <c r="R31" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.4603276196571793</v>
       </c>
       <c r="S31" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.8624717483048983</v>
       </c>
       <c r="T31" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.2200132007920475</v>
       </c>
       <c r="U31" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.19201152069124147</v>
       </c>
       <c r="V31" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.6003360201612104E-2</v>
       </c>
       <c r="W31" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.6000960057603455E-2</v>
       </c>
       <c r="X31" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.3522011320679237</v>
       </c>
       <c r="Y31" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.8582314938896336</v>
       </c>
       <c r="Z31" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.11600696041762507</v>
       </c>
       <c r="AA31" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.12600756045362721</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="27"/>
-        <v>2.9730887933275998</v>
+        <f t="shared" si="28"/>
+        <v>11.476122742244534</v>
       </c>
     </row>
     <row r="32" spans="2:28">
@@ -2987,54 +3097,54 @@
         <v>75</v>
       </c>
       <c r="R32" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.4603276196571793</v>
       </c>
       <c r="S32" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8.2824969498169896</v>
       </c>
       <c r="T32" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.25401524091445482</v>
       </c>
       <c r="U32" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.19801188071284279</v>
       </c>
       <c r="V32" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>3.4002040122407345E-2</v>
       </c>
       <c r="W32" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3.0001800108006477E-2</v>
       </c>
       <c r="X32" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3.1861911714702882</v>
       </c>
       <c r="Y32" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.8982338940336416</v>
       </c>
       <c r="Z32" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>9.8005880352821165E-2</v>
       </c>
       <c r="AA32" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.15000900054003241</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="27"/>
-        <v>3.0156607836470188</v>
+        <f t="shared" si="28"/>
+        <v>11.640450624877493</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="AB25:AB32">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>